<commit_message>
Update Arduino code for Watermark
</commit_message>
<xml_diff>
--- a/Arduino/Intelirris_Soil_Sensor/watermark.xlsx
+++ b/Arduino/Intelirris_Soil_Sensor/watermark.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>&lt;550</t>
   </si>
@@ -55,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -94,7 +94,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,69 +372,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="14.83203125" customWidth="1"/>
+    <col min="3" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>5300</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>3589</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="C5" s="2">
-        <f>ABS(($C$2/1000*23.156-12.736)-(1+0.018*($E$2-24)))</f>
-        <v>108.91879999999998</v>
-      </c>
       <c r="D5" s="2">
-        <f>ABS((-3.213*($C$2/1000)-4.093)/(1-0.009733*($C$2/1000)-0.01205*($E$2)))</f>
-        <v>34.568540122821844</v>
+        <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A5-24)))</f>
+        <v>69.298883999999987</v>
       </c>
       <c r="E5" s="2">
-        <f>ABS(2.246-5.239*($C$2/1000)*(1+0.018*($E$2-24))-0.06756*($C$2/1000)*($C$2/1000)*((1+0.018*($E$2-24))*(1+0.018*($E$2-24))))</f>
-        <v>29.700778287513604</v>
+        <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A5)))</f>
+        <v>24.892858092460216</v>
+      </c>
+      <c r="F5" s="2">
+        <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A5-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A5-24))*(1+0.018*($A5-24))))</f>
+        <v>18.910630676395431</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="C8" s="1"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A6-24)))</f>
+        <v>69.442883999999992</v>
+      </c>
+      <c r="E6" s="2">
+        <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A6)))</f>
+        <v>21.578707144632851</v>
+      </c>
+      <c r="F6" s="2">
+        <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A6-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A6-24))*(1+0.018*($A6-24))))</f>
+        <v>15.952403965840549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Arduino code for wm+soil temperature
</commit_message>
<xml_diff>
--- a/Arduino/Intelirris_Soil_Sensor/watermark.xlsx
+++ b/Arduino/Intelirris_Soil_Sensor/watermark.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1140" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="2660" yWindow="1960" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>&lt;550</t>
   </si>
@@ -41,13 +41,25 @@
     <t>&gt;8000</t>
   </si>
   <si>
-    <t>R=</t>
-  </si>
-  <si>
     <t>T=</t>
   </si>
   <si>
     <t>CB</t>
+  </si>
+  <si>
+    <t>default in INTEL-IRRIS soil sensor devicde</t>
+  </si>
+  <si>
+    <t>default in Irrometer calibration table: https://www.irrometer.com/download/caltable.xls</t>
+  </si>
+  <si>
+    <t>add your own temperature to test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R=</t>
+  </si>
+  <si>
+    <t>enter read resistance --&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -57,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,21 +77,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF5B5B5B"/>
-      <name val="Lato"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,14 +136,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -383,40 +462,41 @@
     <col min="3" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15"/>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>3589</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="2">
         <f>0</f>
@@ -424,46 +504,90 @@
       </c>
       <c r="D5" s="2">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A5-24)))</f>
-        <v>69.298883999999987</v>
+        <v>2.0538599999999994</v>
       </c>
       <c r="E5" s="2">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A5)))</f>
-        <v>24.892858092460216</v>
+        <v>9.5953489266611633</v>
       </c>
       <c r="F5" s="2">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A5-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A5-24))*(1+0.018*($A5-24))))</f>
-        <v>18.910630676395431</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
+        <v>1.6375325792637443</v>
+      </c>
+      <c r="G5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A6-24)))</f>
-        <v>69.442883999999992</v>
-      </c>
-      <c r="E6" s="2">
+        <v>2.1258599999999994</v>
+      </c>
+      <c r="E6" s="4">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A6)))</f>
-        <v>21.578707144632851</v>
-      </c>
-      <c r="F6" s="2">
+        <v>8.9385186300662749</v>
+      </c>
+      <c r="F6" s="4">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A6-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A6-24))*(1+0.018*($A6-24))))</f>
-        <v>15.952403965840549</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+        <v>1.374415841</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>24.9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A7-24)))</f>
+        <v>2.1096599999999994</v>
+      </c>
+      <c r="E7" s="6">
+        <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A7)))</f>
+        <v>9.0783425549352774</v>
+      </c>
+      <c r="F7" s="6">
+        <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A7-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A7-24))*(1+0.018*($A7-24))))</f>
+        <v>1.4335884508171122</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update soil sensor code and PCBs description
</commit_message>
<xml_diff>
--- a/Arduino/Intelirris_Soil_Sensor/watermark.xlsx
+++ b/Arduino/Intelirris_Soil_Sensor/watermark.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpham/Dropbox (Compte personnel)/Arduino/sketch/00-PRIMA-Intel-Irris/Intelirris_Soil_Sensor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpham/Library/CloudStorage/GoogleDrive-congduc.pham@waziup.org/Mon Drive/Arduino/sketch/00-PRIMA-Intel-Irris/Intelirris_Soil_Sensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A053E8-30A8-3C47-9357-FA53031BEB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1960" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="3180" yWindow="1940" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -65,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -183,6 +195,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -450,7 +465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -471,7 +486,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="7">
-        <v>685</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -504,15 +519,15 @@
       </c>
       <c r="D5" s="2">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A5-24)))</f>
-        <v>2.0538599999999994</v>
+        <v>10.366864</v>
       </c>
       <c r="E5" s="2">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A5)))</f>
-        <v>9.5953489266611633</v>
+        <v>11.414668461720485</v>
       </c>
       <c r="F5" s="2">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A5-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A5-24))*(1+0.018*($A5-24))))</f>
-        <v>1.6375325792637443</v>
+        <v>3.7019425525458547</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -531,15 +546,15 @@
       </c>
       <c r="D6" s="4">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A6-24)))</f>
-        <v>2.1258599999999994</v>
+        <v>10.438863999999999</v>
       </c>
       <c r="E6" s="4">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A6)))</f>
-        <v>8.9385186300662749</v>
+        <v>10.629403556767031</v>
       </c>
       <c r="F6" s="4">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A6-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A6-24))*(1+0.018*($A6-24))))</f>
-        <v>1.374415841</v>
+        <v>3.2971520761600006</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -547,7 +562,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
-        <v>24.9</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>5</v>
@@ -558,15 +573,15 @@
       </c>
       <c r="D7" s="6">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A7-24)))</f>
-        <v>2.1096599999999994</v>
+        <v>10.708863999999998</v>
       </c>
       <c r="E7" s="6">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A7)))</f>
-        <v>9.0783425549352774</v>
+        <v>8.4495882400350304</v>
       </c>
       <c r="F7" s="6">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A7-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A7-24))*(1+0.018*($A7-24))))</f>
-        <v>1.4335884508171122</v>
+        <v>1.7859873449856642</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>

</xml_diff>